<commit_message>
Forgot to commit these
</commit_message>
<xml_diff>
--- a/+aae550/+hw1/partII_a.xlsx
+++ b/+aae550/+hw1/partII_a.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12330"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13770"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -485,43 +485,43 @@
         <v>18</v>
       </c>
       <c r="E2">
-        <v>312.25281401069935</v>
+        <v>312.25115369684761</v>
       </c>
       <c r="F2">
-        <v>-8.0318613115462174</v>
+        <v>-8.0318491234546219</v>
       </c>
       <c r="G2">
-        <v>-9.6813868845378237E-2</v>
+        <v>-9.6815087654537724E-2</v>
       </c>
       <c r="H2">
-        <v>-10.112069469034616</v>
+        <v>-10.112054942940608</v>
       </c>
       <c r="I2">
-        <v>-1.2260491641367444E-2</v>
+        <v>-1.226178284972379E-2</v>
       </c>
       <c r="J2">
-        <v>5.0210616834269084E-2</v>
+        <v>5.0213410604839082E-2</v>
       </c>
       <c r="K2">
-        <v>-0.42205736318524734</v>
+        <v>-0.42205169102136431</v>
       </c>
       <c r="L2">
-        <v>-0.64448565920368817</v>
+        <v>-0.64448707724465892</v>
       </c>
       <c r="M2">
-        <v>-0.55398014705226339</v>
+        <v>-0.55397777535873804</v>
       </c>
       <c r="N2">
-        <v>9.5138099573274459E-2</v>
+        <v>9.514535503055277E-2</v>
       </c>
       <c r="O2">
-        <v>-0.34632464931463447</v>
+        <v>-0.34631943650294505</v>
       </c>
       <c r="P2">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="Q2">
-        <v>5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
@@ -538,37 +538,37 @@
         <v>19</v>
       </c>
       <c r="E3">
-        <v>331.28137597847348</v>
+        <v>331.28137564737455</v>
       </c>
       <c r="F3">
-        <v>-8.130520040192188</v>
+        <v>-8.1305200810389877</v>
       </c>
       <c r="G3">
-        <v>-8.6947995980781068E-2</v>
+        <v>-8.694799189610114E-2</v>
       </c>
       <c r="H3">
-        <v>-10.226541273331963</v>
+        <v>-10.226541325427219</v>
       </c>
       <c r="I3">
-        <v>-2.0852201482699506E-3</v>
+        <v>-2.0852155175806741E-3</v>
       </c>
       <c r="J3">
-        <v>1.1014044938727041E-2</v>
+        <v>1.1014055162195335E-2</v>
       </c>
       <c r="K3">
-        <v>-0.49287021526618435</v>
+        <v>-0.49287020697214112</v>
       </c>
       <c r="L3">
-        <v>-0.62678244618345391</v>
+        <v>-0.62678244825696472</v>
       </c>
       <c r="M3">
-        <v>-0.57960059860982416</v>
+        <v>-0.57960059818927179</v>
       </c>
       <c r="N3">
-        <v>2.1698781706808168E-2</v>
+        <v>2.1698777989694884E-2</v>
       </c>
       <c r="O3">
-        <v>-0.39674928961930667</v>
+        <v>-0.39674929451277063</v>
       </c>
       <c r="P3">
         <v>17</v>
@@ -591,37 +591,37 @@
         <v>20</v>
       </c>
       <c r="E4">
-        <v>336.24534792015163</v>
+        <v>336.24534636048384</v>
       </c>
       <c r="F4">
-        <v>-8.1316532494542244</v>
+        <v>-8.1316532899987468</v>
       </c>
       <c r="G4">
-        <v>-8.6834675054577537E-2</v>
+        <v>-8.6834671000125319E-2</v>
       </c>
       <c r="H4">
-        <v>-10.225161920688686</v>
+        <v>-10.225161973110446</v>
       </c>
       <c r="I4">
-        <v>-2.2078292721168236E-3</v>
+        <v>-2.2078246124047629E-3</v>
       </c>
       <c r="J4">
-        <v>-3.9082310961032762E-3</v>
+        <v>-3.9082174032528672E-3</v>
       </c>
       <c r="K4">
-        <v>-0.51523712903275376</v>
+        <v>-0.51523711510389569</v>
       </c>
       <c r="L4">
-        <v>-0.62119071774181156</v>
+        <v>-0.62119072122402608</v>
       </c>
       <c r="M4">
-        <v>-0.58580749854618852</v>
+        <v>-0.58580749662443465</v>
       </c>
       <c r="N4">
-        <v>6.7350617239834154E-3</v>
+        <v>6.7350616961001641E-3</v>
       </c>
       <c r="O4">
-        <v>-0.40565821715545181</v>
+        <v>-0.40565821981078953</v>
       </c>
       <c r="P4">
         <v>4</v>
@@ -644,37 +644,37 @@
         <v>21</v>
       </c>
       <c r="E5">
-        <v>338.06386594055181</v>
+        <v>338.06386436367933</v>
       </c>
       <c r="F5">
-        <v>-8.1320723650185389</v>
+        <v>-8.1320724055571301</v>
       </c>
       <c r="G5">
-        <v>-8.679276349814613E-2</v>
+        <v>-8.6792759444286882E-2</v>
       </c>
       <c r="H5">
-        <v>-10.224661655476808</v>
+        <v>-10.224661707905506</v>
       </c>
       <c r="I5">
-        <v>-2.2522972909503336E-3</v>
+        <v>-2.2522926306216551E-3</v>
       </c>
       <c r="J5">
-        <v>-9.2643542244508215E-3</v>
+        <v>-9.2643405795790335E-3</v>
       </c>
       <c r="K5">
-        <v>-0.52343040637091809</v>
+        <v>-0.52343039232726296</v>
       </c>
       <c r="L5">
-        <v>-0.61914239840727048</v>
+        <v>-0.61914240191818426</v>
       </c>
       <c r="M5">
-        <v>-0.58803573720269053</v>
+        <v>-0.58803573528058151</v>
       </c>
       <c r="N5">
-        <v>1.3627254902826014E-3</v>
+        <v>1.362725487747074E-3</v>
       </c>
       <c r="O5">
-        <v>-0.4088569915368967</v>
+        <v>-0.40885699416256294</v>
       </c>
       <c r="P5">
         <v>3</v>
@@ -697,37 +697,37 @@
         <v>22</v>
       </c>
       <c r="E6">
-        <v>338.48756233707343</v>
+        <v>338.48756076366965</v>
       </c>
       <c r="F6">
-        <v>-8.1321697487697637</v>
+        <v>-8.1321697893086604</v>
       </c>
       <c r="G6">
-        <v>-8.6783025123023494E-2</v>
+        <v>-8.6783021069133937E-2</v>
       </c>
       <c r="H6">
-        <v>-10.224544760933416</v>
+        <v>-10.224544813361623</v>
       </c>
       <c r="I6">
-        <v>-2.2626879170296599E-3</v>
+        <v>-2.2626832567445021E-3</v>
       </c>
       <c r="J6">
-        <v>-1.0504069084466106E-2</v>
+        <v>-1.0504055472598472E-2</v>
       </c>
       <c r="K6">
-        <v>-0.52533940023031889</v>
+        <v>-0.52533938619361376</v>
       </c>
       <c r="L6">
-        <v>-0.61866514994242028</v>
+        <v>-0.61866515345159656</v>
       </c>
       <c r="M6">
-        <v>-0.58855145553832444</v>
+        <v>-0.58855145362523897</v>
       </c>
       <c r="N6">
-        <v>1.193462059736472E-4</v>
+        <v>1.1934618735454094E-4</v>
       </c>
       <c r="O6">
-        <v>-0.40959730225827851</v>
+        <v>-0.40959730489014479</v>
       </c>
       <c r="P6">
         <v>2</v>
@@ -750,37 +750,37 @@
         <v>22</v>
       </c>
       <c r="E7">
-        <v>338.52904210527026</v>
+        <v>338.5290405049563</v>
       </c>
       <c r="F7">
-        <v>-8.1321791816149656</v>
+        <v>-8.1321792221476752</v>
       </c>
       <c r="G7">
-        <v>-8.6782081838503444E-2</v>
+        <v>-8.6782077785232503E-2</v>
       </c>
       <c r="H7">
-        <v>-10.224533188599679</v>
+        <v>-10.224533241035418</v>
       </c>
       <c r="I7">
-        <v>-2.2637165689174399E-3</v>
+        <v>-2.2637119079628176E-3</v>
       </c>
       <c r="J7">
-        <v>-1.0625292333237502E-2</v>
+        <v>-1.0625278644965541E-2</v>
       </c>
       <c r="K7">
-        <v>-0.52552630735222072</v>
+        <v>-0.52552629319340216</v>
       </c>
       <c r="L7">
-        <v>-0.61861842316194482</v>
+        <v>-0.61861842670164946</v>
       </c>
       <c r="M7">
-        <v>-0.58860187485780835</v>
+        <v>-0.58860187291248312</v>
       </c>
       <c r="N7">
-        <v>-2.2016212376518851E-6</v>
+        <v>-2.20156157948459E-6</v>
       </c>
       <c r="O7">
-        <v>-0.40966966562672935</v>
+        <v>-0.40966966821166217</v>
       </c>
       <c r="P7">
         <v>1</v>
@@ -803,37 +803,37 @@
         <v>22</v>
       </c>
       <c r="E8">
-        <v>338.52440808943913</v>
+        <v>338.52440651440168</v>
       </c>
       <c r="F8">
-        <v>-8.1321781287731003</v>
+        <v>-8.1321781693115582</v>
       </c>
       <c r="G8">
-        <v>-8.6782187122689924E-2</v>
+        <v>-8.678218306884411E-2</v>
       </c>
       <c r="H8">
-        <v>-10.224534482667417</v>
+        <v>-10.224534535096094</v>
       </c>
       <c r="I8">
-        <v>-2.263601540673954E-3</v>
+        <v>-2.2635968803472739E-3</v>
       </c>
       <c r="J8">
-        <v>-1.0611750835283096E-2</v>
+        <v>-1.0611737220627471E-2</v>
       </c>
       <c r="K8">
-        <v>-0.52550542639166009</v>
+        <v>-0.52550541234683923</v>
       </c>
       <c r="L8">
-        <v>-0.61862364340208498</v>
+        <v>-0.61862364691329019</v>
       </c>
       <c r="M8">
-        <v>-0.58859624275073286</v>
+        <v>-0.58859624083607764</v>
       </c>
       <c r="N8">
-        <v>1.1375809765068468E-5</v>
+        <v>1.1375795425205837E-5</v>
       </c>
       <c r="O8">
-        <v>-0.40966158238004013</v>
+        <v>-0.40966158500906424</v>
       </c>
       <c r="P8">
         <v>1</v>
@@ -856,37 +856,37 @@
         <v>22</v>
       </c>
       <c r="E9">
-        <v>338.53162970240624</v>
+        <v>338.53162810627509</v>
       </c>
       <c r="F9">
-        <v>-8.1321796160316726</v>
+        <v>-8.1321796565655156</v>
       </c>
       <c r="G9">
-        <v>-8.6782038396832739E-2</v>
+        <v>-8.6782034343448444E-2</v>
       </c>
       <c r="H9">
-        <v>-10.224532270891176</v>
+        <v>-10.224532323325988</v>
       </c>
       <c r="I9">
-        <v>-2.2637981430064791E-3</v>
+        <v>-2.2637934821344574E-3</v>
       </c>
       <c r="J9">
-        <v>-1.0632887456335505E-2</v>
+        <v>-1.0632873780386021E-2</v>
       </c>
       <c r="K9">
-        <v>-0.5255379931873092</v>
+        <v>-0.52553797904725341</v>
       </c>
       <c r="L9">
-        <v>-0.6186155017031727</v>
+        <v>-0.61861550523818665</v>
       </c>
       <c r="M9">
-        <v>-0.58860501971530454</v>
+        <v>-0.58860501777509322</v>
       </c>
       <c r="N9">
-        <v>-9.765614965573377E-6</v>
+        <v>-9.7655676213337372E-6</v>
       </c>
       <c r="O9">
-        <v>-0.40967415897323856</v>
+        <v>-0.40967416156549408</v>
       </c>
       <c r="P9">
         <v>1</v>
@@ -909,37 +909,37 @@
         <v>22</v>
       </c>
       <c r="E10">
-        <v>338.52836095123666</v>
+        <v>338.5283593748498</v>
       </c>
       <c r="F10">
-        <v>-8.1321788733759544</v>
+        <v>-8.1321789139142879</v>
       </c>
       <c r="G10">
-        <v>-8.6782112662404431E-2</v>
+        <v>-8.6782108608571162E-2</v>
       </c>
       <c r="H10">
-        <v>-10.224533183703169</v>
+        <v>-10.224533236132462</v>
       </c>
       <c r="I10">
-        <v>-2.2637170041627241E-3</v>
+        <v>-2.263712343781088E-3</v>
       </c>
       <c r="J10">
-        <v>-1.0623335712848347E-2</v>
+        <v>-1.062332209442074E-2</v>
       </c>
       <c r="K10">
-        <v>-0.5255232641341987</v>
+        <v>-0.52552325008318279</v>
       </c>
       <c r="L10">
-        <v>-0.61861918396645033</v>
+        <v>-0.6186191874792043</v>
       </c>
       <c r="M10">
-        <v>-0.588601047005328</v>
+        <v>-0.58860104508907696</v>
       </c>
       <c r="N10">
-        <v>-1.8852492433829582E-7</v>
+        <v>-1.8853538563678995E-7</v>
       </c>
       <c r="O10">
-        <v>-0.40966845730679602</v>
+        <v>-0.40966845993349155</v>
       </c>
       <c r="P10">
         <v>1</v>
@@ -962,37 +962,37 @@
         <v>22</v>
       </c>
       <c r="E11">
-        <v>338.52836095123666</v>
+        <v>338.5283593748498</v>
       </c>
       <c r="F11">
-        <v>-8.1321788733759544</v>
+        <v>-8.1321789139142879</v>
       </c>
       <c r="G11">
-        <v>-8.6782112662404431E-2</v>
+        <v>-8.6782108608571162E-2</v>
       </c>
       <c r="H11">
-        <v>-10.224533183703169</v>
+        <v>-10.224533236132462</v>
       </c>
       <c r="I11">
-        <v>-2.2637170041627241E-3</v>
+        <v>-2.263712343781088E-3</v>
       </c>
       <c r="J11">
-        <v>-1.0623335712848347E-2</v>
+        <v>-1.062332209442074E-2</v>
       </c>
       <c r="K11">
-        <v>-0.5255232641341987</v>
+        <v>-0.52552325008318279</v>
       </c>
       <c r="L11">
-        <v>-0.61861918396645033</v>
+        <v>-0.6186191874792043</v>
       </c>
       <c r="M11">
-        <v>-0.588601047005328</v>
+        <v>-0.58860104508907696</v>
       </c>
       <c r="N11">
-        <v>-1.8852492433829582E-7</v>
+        <v>-1.8853538563678995E-7</v>
       </c>
       <c r="O11">
-        <v>-0.40966845730679602</v>
+        <v>-0.40966845993349155</v>
       </c>
       <c r="P11">
         <v>1</v>

</xml_diff>